<commit_message>
edit funnel and timeline chart documentation
</commit_message>
<xml_diff>
--- a/visual/sample-data/timeline-chart/US-president-death.xlsx
+++ b/visual/sample-data/timeline-chart/US-president-death.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.syafiq\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.syafiq\Desktop\timeline-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Number</t>
   </si>
@@ -111,16 +111,54 @@
   </si>
   <si>
     <t>Cerebral hemorrhage</t>
+  </si>
+  <si>
+    <t>Image of President</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/William_mckinley.jpg/220px-William_mckinley.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/c/c5/William_Henry_Harrison_daguerreotype_edit.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/a/ab/Abraham_Lincoln_O-77_matte_collodion_print.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/1/1f/James_Abram_Garfield%2C_photo_portrait_seated.jpg/1200px-James_Abram_Garfield%2C_photo_portrait_seated.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c4/Warren_G_Harding-Harris_%26_Ewing.jpg/1200px-Warren_G_Harding-Harris_%26_Ewing.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c3/John_F._Kennedy%2C_White_House_color_photo_portrait.jpg/1200px-John_F._Kennedy%2C_White_House_color_photo_portrait.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/1/16/Official_Portrait_of_President_Reagan_1981.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/d/d4/George-W-Bush.jpeg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/42/FDR_1944_Color_Portrait.jpg/1200px-FDR_1944_Color_Portrait.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,17 +181,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,10 +484,12 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +508,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -485,8 +531,11 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -505,8 +554,11 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -525,8 +577,11 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -545,8 +600,11 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -565,9 +623,12 @@
       <c r="F6" t="s">
         <v>19</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -586,9 +647,12 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -607,9 +671,12 @@
       <c r="F8" t="s">
         <v>23</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -628,9 +695,12 @@
       <c r="F9" t="s">
         <v>25</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -649,8 +719,24 @@
       <c r="F10" t="s">
         <v>28</v>
       </c>
-    </row>
+      <c r="G10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>